<commit_message>
Update evaluation with Olivier's batch
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31560" windowHeight="19780" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="20060" windowHeight="19040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>Aghamahdi Mohammad Hossein</t>
   </si>
@@ -235,13 +235,16 @@
   </si>
   <si>
     <t>18/05/2016 (Olivier)</t>
+  </si>
+  <si>
+    <t>25/05/2016 (Olivier)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -307,8 +310,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +334,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -352,7 +368,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -376,8 +392,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -397,8 +433,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="43">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -410,6 +447,16 @@
     <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -421,9 +468,179 @@
     <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -773,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -922,14 +1139,16 @@
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="1"/>
@@ -949,7 +1168,7 @@
       </c>
       <c r="L5" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -959,47 +1178,57 @@
       <c r="B6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="C6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="1"/>
@@ -1019,7 +1248,7 @@
       </c>
       <c r="L7" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1062,14 +1291,16 @@
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
@@ -1089,7 +1320,7 @@
       </c>
       <c r="L9" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1130,14 +1361,16 @@
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="1"/>
@@ -1157,21 +1390,23 @@
       </c>
       <c r="L11" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="1"/>
@@ -1191,25 +1426,29 @@
       </c>
       <c r="L12" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="2"/>
@@ -1225,7 +1464,7 @@
       </c>
       <c r="L13" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1266,14 +1505,16 @@
       <c r="A15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="1"/>
@@ -1293,21 +1534,23 @@
       </c>
       <c r="L15" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="1"/>
@@ -1327,7 +1570,7 @@
       </c>
       <c r="L16" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1373,9 +1616,15 @@
       <c r="B18" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="5">
         <f t="shared" si="0"/>
@@ -1383,15 +1632,15 @@
       </c>
       <c r="H18" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="4"/>
@@ -1399,7 +1648,7 @@
       </c>
       <c r="L18" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1440,14 +1689,16 @@
       <c r="A20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="1"/>
@@ -1467,29 +1718,35 @@
       </c>
       <c r="L20" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="B21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="5">
         <f t="shared" si="3"/>
@@ -1501,21 +1758,23 @@
       </c>
       <c r="L21" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="1"/>
@@ -1535,7 +1794,7 @@
       </c>
       <c r="L22" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1576,14 +1835,16 @@
       <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="5">
         <f t="shared" si="1"/>
@@ -1603,21 +1864,23 @@
       </c>
       <c r="L24" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5">
         <f t="shared" si="1"/>
@@ -1637,7 +1900,7 @@
       </c>
       <c r="L25" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1714,14 +1977,16 @@
       <c r="A28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="5">
         <f t="shared" si="1"/>
@@ -1741,7 +2006,7 @@
       </c>
       <c r="L28" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1920,14 +2185,16 @@
       <c r="A34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5">
         <f t="shared" si="1"/>
@@ -1947,21 +2214,23 @@
       </c>
       <c r="L34" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="7"/>
+      <c r="B35" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5">
         <f t="shared" si="1"/>
@@ -1981,7 +2250,7 @@
       </c>
       <c r="L35" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2024,14 +2293,16 @@
       <c r="A37" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="7"/>
+      <c r="B37" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="5">
         <f t="shared" si="1"/>
@@ -2051,21 +2322,23 @@
       </c>
       <c r="L37" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="5">
         <f t="shared" si="1"/>
@@ -2085,25 +2358,29 @@
       </c>
       <c r="L38" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
+      <c r="B39" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="5">
         <f t="shared" si="2"/>
@@ -2119,7 +2396,7 @@
       </c>
       <c r="L39" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2160,14 +2437,16 @@
       <c r="A41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="7"/>
+      <c r="B41" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="5">
         <f t="shared" si="1"/>
@@ -2187,21 +2466,23 @@
       </c>
       <c r="L41" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="7"/>
+      <c r="B42" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="5">
         <f t="shared" si="1"/>
@@ -2221,21 +2502,23 @@
       </c>
       <c r="L42" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="7"/>
+      <c r="B43" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="5">
         <f t="shared" si="1"/>
@@ -2255,21 +2538,23 @@
       </c>
       <c r="L43" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="7"/>
+      <c r="B44" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="5">
         <f t="shared" si="1"/>
@@ -2289,29 +2574,35 @@
       </c>
       <c r="L44" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
+      <c r="B45" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="5">
         <f t="shared" si="3"/>
@@ -2323,7 +2614,7 @@
       </c>
       <c r="L45" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2398,14 +2689,16 @@
       <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="7"/>
+      <c r="B48" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="5">
         <f t="shared" si="1"/>
@@ -2425,21 +2718,23 @@
       </c>
       <c r="L48" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="7"/>
+      <c r="B49" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="5">
         <f t="shared" si="1"/>
@@ -2459,21 +2754,23 @@
       </c>
       <c r="L49" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="7"/>
+      <c r="B50" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="5">
         <f t="shared" si="1"/>
@@ -2493,21 +2790,23 @@
       </c>
       <c r="L50" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="7"/>
+      <c r="B51" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="5">
         <f t="shared" si="1"/>
@@ -2527,21 +2826,23 @@
       </c>
       <c r="L51" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="7"/>
+      <c r="B52" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" s="5">
         <f t="shared" si="1"/>
@@ -2561,21 +2862,23 @@
       </c>
       <c r="L52" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="7"/>
+      <c r="B53" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" s="5">
         <f t="shared" si="1"/>
@@ -2595,7 +2898,7 @@
       </c>
       <c r="L53" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -2706,11 +3009,11 @@
   <sortState ref="A2:H56">
     <sortCondition ref="A2:A56"/>
   </sortState>
-  <conditionalFormatting sqref="B3:F56">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B46:F47 E45:F45 B54:F56 B26:F33 B23:F23 E21:F21 C41:F44 B3:F4 B8:F8 B6 C7:F7 B19:F19 B18 F18 B36:F36 B17:F17 B14:F14 B39:F40 C34:F35 C11:F12 D13:F13 C5:F5 C24:F25 B10:F10 C9:F9 C22:F22 C37:F38 C15:F16 C48:F53 C20:F20">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="1">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="16" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Phase 1 evaluation done.
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="18340" windowHeight="19040" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="20060" windowHeight="19040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
   <si>
     <t>Aghamahdi Mohammad Hossein</t>
   </si>
@@ -381,8 +381,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -453,7 +455,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -477,6 +479,7 @@
     <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -500,9 +503,30 @@
     <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -992,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2078,14 +2102,16 @@
       <c r="A30" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" si="1"/>
@@ -2105,7 +2131,7 @@
       </c>
       <c r="L30" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -3054,67 +3080,67 @@
   <sortState ref="A2:H56">
     <sortCondition ref="A2:A56"/>
   </sortState>
-  <conditionalFormatting sqref="B47:F47 E45:F45 B55:F55 B27:F28 E21:F21 B4:F4 B8:F8 B6 C7:F7 B36:F36 B17:B18 F14 B39:F39 D13:F13 C5:F5 C9:F12 C37:F38 C15:F16 C48:F51 C19:F20 C3:F3 F17:F18 C22:F26 B30:F31 C29:F29 C32:F35 C40:F44 C46:F46 D52:F52 C53:F54 C56:F56">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="17">
+  <conditionalFormatting sqref="B47:F47 E45:F45 B55:F55 B27:F28 E21:F21 B4:F4 B8:F8 B6 C7:F7 B36:F36 B17:B18 F14 B39:F39 D13:F13 C5:F5 C9:F12 C37:F38 C15:F16 C48:F51 C19:F20 C3:F3 F17:F18 C22:F26 C29:F29 C32:F35 C40:F44 C46:F46 D52:F52 C53:F54 C56:F56 B30:F31">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="17">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="14" priority="18">
+    <cfRule type="containsBlanks" dxfId="16" priority="18">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="15">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="12" priority="16">
+    <cfRule type="containsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="13">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="10" priority="14">
+    <cfRule type="containsBlanks" dxfId="12" priority="14">
       <formula>LEN(TRIM(B10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:E14">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="11">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="8" priority="12">
+    <cfRule type="containsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(B14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:D17">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
       <formula>LEN(TRIM(C17))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="6" priority="10">
+    <cfRule type="containsBlanks" dxfId="8" priority="10">
       <formula>LEN(TRIM(C17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(B46))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(B46))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(B54))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(B54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(B29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding new batch, validated by Olivier
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
   <si>
     <t>Aghamahdi Mohammad Hossein</t>
   </si>
@@ -396,8 +396,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -478,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -506,6 +508,7 @@
     <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -533,6 +536,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -1025,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1183,8 +1187,12 @@
       <c r="B5" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="5">
@@ -1193,11 +1201,11 @@
       </c>
       <c r="H5" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="3"/>
@@ -1209,7 +1217,7 @@
       </c>
       <c r="L5" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1263,7 +1271,9 @@
       <c r="B7" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1273,7 +1283,7 @@
       </c>
       <c r="H7" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="2"/>
@@ -1289,7 +1299,7 @@
       </c>
       <c r="L7" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1371,7 +1381,9 @@
       <c r="B10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1381,7 +1393,7 @@
       </c>
       <c r="H10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="2"/>
@@ -1397,7 +1409,7 @@
       </c>
       <c r="L10" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1407,7 +1419,9 @@
       <c r="B11" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1417,7 +1431,7 @@
       </c>
       <c r="H11" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="2"/>
@@ -1433,7 +1447,7 @@
       </c>
       <c r="L11" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1443,7 +1457,9 @@
       <c r="B12" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -1453,7 +1469,7 @@
       </c>
       <c r="H12" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="2"/>
@@ -1469,7 +1485,7 @@
       </c>
       <c r="L12" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1511,7 +1527,7 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1526,7 +1542,9 @@
       <c r="E14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1545,11 +1563,11 @@
       </c>
       <c r="K14" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M14" s="14" t="s">
         <v>74</v>
@@ -1598,7 +1616,9 @@
       <c r="B16" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1608,7 +1628,7 @@
       </c>
       <c r="H16" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="2"/>
@@ -1624,7 +1644,7 @@
       </c>
       <c r="L16" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2020,7 +2040,9 @@
       <c r="B27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2030,7 +2052,7 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="2"/>
@@ -2046,7 +2068,7 @@
       </c>
       <c r="L27" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2130,7 +2152,9 @@
       <c r="B30" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="7"/>
+      <c r="C30" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2140,7 +2164,7 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" si="2"/>
@@ -2156,7 +2180,7 @@
       </c>
       <c r="L30" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2166,7 +2190,9 @@
       <c r="B31" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="7"/>
+      <c r="C31" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2176,7 +2202,7 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" si="2"/>
@@ -2192,7 +2218,7 @@
       </c>
       <c r="L31" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2276,7 +2302,9 @@
       <c r="B34" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2286,7 +2314,7 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="5">
         <f t="shared" si="2"/>
@@ -2302,7 +2330,7 @@
       </c>
       <c r="L34" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2422,7 +2450,9 @@
       <c r="B38" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2432,7 +2462,7 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="5">
         <f t="shared" si="2"/>
@@ -2448,7 +2478,7 @@
       </c>
       <c r="L38" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2496,7 +2526,9 @@
       <c r="B40" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -2506,7 +2538,7 @@
       </c>
       <c r="H40" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="5">
         <f t="shared" si="2"/>
@@ -2522,7 +2554,7 @@
       </c>
       <c r="L40" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2562,39 +2594,47 @@
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="G42" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H42" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2642,7 +2682,9 @@
       <c r="B44" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
@@ -2652,7 +2694,7 @@
       </c>
       <c r="H44" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="5">
         <f t="shared" si="2"/>
@@ -2668,7 +2710,7 @@
       </c>
       <c r="L44" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2978,7 +3020,9 @@
       <c r="B53" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="7"/>
+      <c r="C53" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
@@ -2988,7 +3032,7 @@
       </c>
       <c r="H53" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="5">
         <f t="shared" si="2"/>
@@ -3004,7 +3048,7 @@
       </c>
       <c r="L53" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3014,7 +3058,9 @@
       <c r="B54" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C54" s="7"/>
+      <c r="C54" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
@@ -3024,7 +3070,7 @@
       </c>
       <c r="H54" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="5">
         <f t="shared" si="2"/>
@@ -3040,7 +3086,7 @@
       </c>
       <c r="L54" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3121,7 +3167,7 @@
   <sortState ref="A2:H56">
     <sortCondition ref="A2:A56"/>
   </sortState>
-  <conditionalFormatting sqref="B47:F47 B55 B27:F27 B4 B8:F8 B6 C7:F7 B36:F36 B17:B18 F14 B39:F39 D13:F13 C5:F5 C9:F12 C37:F38 C15:F16 C48:F48 C20:F20 F18 C22:F23 C29:F29 C32:F32 C40:F42 E45:F45 D52:F52 C53:F54 C56:F56 B30:F31 C25:F26 D24:F24 D19:F19 C34:F34 D33:F33 D55:F55 B28 D28:F28 C44:F44 D43:F43 D35:F35 F46 D3:F4 C50:F51 D49:F49">
+  <conditionalFormatting sqref="B47:F47 B55 B27:F27 B4 B8:F8 B6 C7:F7 B36:F36 B17:B18 F14 B39:F39 D13:F13 C5:F5 C9:F12 C37:F38 C15:F16 C48:F48 C20:F20 F18 C22:F23 C29:F29 C32:F32 C40:F42 E45:F45 D52:F52 C53:F54 C56:F56 B30:F30 C25:F26 D24:F24 D19:F19 C34:F34 D33:F33 D55:F55 B28 D28:F28 C44:F44 D43:F43 D35:F35 F46 D3:F4 C50:F51 D49:F49 B31 D31:F31">
     <cfRule type="notContainsBlanks" dxfId="15" priority="17">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
All evaluations for steps 3 & 4.
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="1720" windowWidth="35120" windowHeight="19380" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="1280" windowWidth="19240" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterateDelta="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="82">
   <si>
     <t>Aghamahdi Mohammad Hossein</t>
   </si>
@@ -250,6 +250,22 @@
   </si>
   <si>
     <t>01/06/2016 (Simon)</t>
+  </si>
+  <si>
+    <t>Problème de configuration Apache à régler.</t>
+  </si>
+  <si>
+    <t>08/06/2016 (Simon)</t>
+  </si>
+  <si>
+    <t>08/06/2016 (Laurent)</t>
+  </si>
+  <si>
+    <t>Sticky session -&gt; OK
+Load Balancing -&gt; OK</t>
+  </si>
+  <si>
+    <t>Question sur AJAX non répondue correctement</t>
   </si>
 </sst>
 </file>
@@ -399,7 +415,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -467,8 +483,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -492,8 +542,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -527,6 +580,23 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -560,9 +630,1586 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="176">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1093,7 +2740,7 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1103,6 +2750,7 @@
     <col min="7" max="7" width="3.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1177,8 +2825,12 @@
       <c r="C3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G56" si="0">IF(B3&lt;&gt;"",1,0)</f>
@@ -1190,11 +2842,11 @@
       </c>
       <c r="I3" s="5">
         <f t="shared" ref="I3:I56" si="2">IF(D3&lt;&gt;"",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J56" si="3">IF(E3&lt;&gt;"",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ref="K3:K56" si="4">IF(F3&lt;&gt;"",1,0)</f>
@@ -1202,7 +2854,7 @@
       </c>
       <c r="L3" s="6">
         <f t="shared" ref="L3:L56" si="5">SUM(G3:K3)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1215,8 +2867,12 @@
       <c r="C4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5">
         <f t="shared" si="0"/>
@@ -1228,11 +2884,11 @@
       </c>
       <c r="I4" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="4"/>
@@ -1240,7 +2896,7 @@
       </c>
       <c r="L4" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1256,7 +2912,9 @@
       <c r="D5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5">
         <f t="shared" si="0"/>
@@ -1272,7 +2930,7 @@
       </c>
       <c r="J5" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="4"/>
@@ -1280,7 +2938,7 @@
       </c>
       <c r="L5" s="6">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1337,8 +2995,12 @@
       <c r="C7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
@@ -1350,11 +3012,11 @@
       </c>
       <c r="I7" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="4"/>
@@ -1362,7 +3024,7 @@
       </c>
       <c r="L7" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1375,8 +3037,12 @@
       <c r="C8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
@@ -1388,11 +3054,11 @@
       </c>
       <c r="I8" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="4"/>
@@ -1400,7 +3066,7 @@
       </c>
       <c r="L8" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1451,8 +3117,12 @@
       <c r="C10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
@@ -1464,11 +3134,11 @@
       </c>
       <c r="I10" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="4"/>
@@ -1476,7 +3146,7 @@
       </c>
       <c r="L10" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1489,9 +3159,15 @@
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1502,19 +3178,19 @@
       </c>
       <c r="I11" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1527,8 +3203,12 @@
       <c r="C12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
@@ -1540,11 +3220,11 @@
       </c>
       <c r="I12" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="4"/>
@@ -1552,7 +3232,7 @@
       </c>
       <c r="L12" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1565,8 +3245,12 @@
       <c r="C13" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
@@ -1578,11 +3262,11 @@
       </c>
       <c r="I13" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="4"/>
@@ -1590,7 +3274,7 @@
       </c>
       <c r="L13" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1650,8 +3334,12 @@
       <c r="C15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
@@ -1663,11 +3351,11 @@
       </c>
       <c r="I15" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="4"/>
@@ -1675,7 +3363,7 @@
       </c>
       <c r="L15" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1688,8 +3376,12 @@
       <c r="C16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
@@ -1701,11 +3393,11 @@
       </c>
       <c r="I16" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="4"/>
@@ -1713,10 +3405,10 @@
       </c>
       <c r="L16" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" s="15" t="s">
         <v>34</v>
       </c>
@@ -1760,7 +3452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1802,7 +3494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
@@ -1812,8 +3504,12 @@
       <c r="C19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
@@ -1825,11 +3521,11 @@
       </c>
       <c r="I19" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="4"/>
@@ -1837,10 +3533,10 @@
       </c>
       <c r="L19" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20" s="7" t="s">
         <v>6</v>
       </c>
@@ -1876,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" s="15" t="s">
         <v>37</v>
       </c>
@@ -1920,7 +3616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
@@ -1930,9 +3626,15 @@
       <c r="C22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="D22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1943,22 +3645,22 @@
       </c>
       <c r="I22" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:13">
       <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1968,9 +3670,15 @@
       <c r="C23" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G23" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1981,22 +3689,22 @@
       </c>
       <c r="I23" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
@@ -2006,8 +3714,12 @@
       <c r="C24" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="5">
         <f t="shared" si="0"/>
@@ -2019,11 +3731,11 @@
       </c>
       <c r="I24" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="4"/>
@@ -2031,10 +3743,10 @@
       </c>
       <c r="L24" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13">
       <c r="A25" s="7" t="s">
         <v>39</v>
       </c>
@@ -2044,9 +3756,15 @@
       <c r="C25" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2057,22 +3775,22 @@
       </c>
       <c r="I25" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13">
       <c r="A26" s="7" t="s">
         <v>9</v>
       </c>
@@ -2082,8 +3800,12 @@
       <c r="C26" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="5">
         <f t="shared" si="0"/>
@@ -2095,11 +3817,11 @@
       </c>
       <c r="I26" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="4"/>
@@ -2107,10 +3829,10 @@
       </c>
       <c r="L26" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27" s="7" t="s">
         <v>10</v>
       </c>
@@ -2120,8 +3842,12 @@
       <c r="C27" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="D27" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
@@ -2133,11 +3859,11 @@
       </c>
       <c r="I27" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="4"/>
@@ -2145,10 +3871,10 @@
       </c>
       <c r="L27" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28" s="7" t="s">
         <v>11</v>
       </c>
@@ -2158,9 +3884,15 @@
       <c r="C28" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="D28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2171,22 +3903,22 @@
       </c>
       <c r="I28" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29" s="7" t="s">
         <v>12</v>
       </c>
@@ -2196,9 +3928,15 @@
       <c r="C29" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="D29" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2209,22 +3947,22 @@
       </c>
       <c r="I29" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30" s="7" t="s">
         <v>40</v>
       </c>
@@ -2234,8 +3972,12 @@
       <c r="C30" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="D30" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F30" s="7"/>
       <c r="G30" s="5">
         <f t="shared" si="0"/>
@@ -2247,11 +3989,11 @@
       </c>
       <c r="I30" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="4"/>
@@ -2259,10 +4001,13 @@
       </c>
       <c r="L30" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="M30" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13">
       <c r="A31" s="7" t="s">
         <v>41</v>
       </c>
@@ -2272,8 +4017,12 @@
       <c r="C31" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F31" s="7"/>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
@@ -2285,11 +4034,11 @@
       </c>
       <c r="I31" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="4"/>
@@ -2297,10 +4046,10 @@
       </c>
       <c r="L31" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13">
       <c r="A32" s="7" t="s">
         <v>13</v>
       </c>
@@ -2310,8 +4059,12 @@
       <c r="C32" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F32" s="7"/>
       <c r="G32" s="5">
         <f t="shared" si="0"/>
@@ -2323,11 +4076,11 @@
       </c>
       <c r="I32" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="4"/>
@@ -2335,10 +4088,10 @@
       </c>
       <c r="L32" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:13">
       <c r="A33" s="7" t="s">
         <v>14</v>
       </c>
@@ -2348,8 +4101,12 @@
       <c r="C33" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+      <c r="D33" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F33" s="7"/>
       <c r="G33" s="5">
         <f t="shared" si="0"/>
@@ -2361,11 +4118,11 @@
       </c>
       <c r="I33" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="5">
         <f t="shared" si="4"/>
@@ -2373,10 +4130,10 @@
       </c>
       <c r="L33" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:13">
       <c r="A34" s="7" t="s">
         <v>42</v>
       </c>
@@ -2386,9 +4143,15 @@
       <c r="C34" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G34" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2399,22 +4162,22 @@
       </c>
       <c r="I34" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:13">
       <c r="A35" s="7" t="s">
         <v>43</v>
       </c>
@@ -2424,8 +4187,12 @@
       <c r="C35" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="D35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F35" s="7"/>
       <c r="G35" s="5">
         <f t="shared" si="0"/>
@@ -2437,11 +4204,11 @@
       </c>
       <c r="I35" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="5">
         <f t="shared" si="4"/>
@@ -2449,10 +4216,10 @@
       </c>
       <c r="L35" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:13">
       <c r="A36" s="7" t="s">
         <v>15</v>
       </c>
@@ -2462,8 +4229,12 @@
       <c r="C36" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="D36" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F36" s="7"/>
       <c r="G36" s="5">
         <f t="shared" si="0"/>
@@ -2475,11 +4246,11 @@
       </c>
       <c r="I36" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="5">
         <f t="shared" si="4"/>
@@ -2487,10 +4258,10 @@
       </c>
       <c r="L36" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:13">
       <c r="A37" s="7" t="s">
         <v>16</v>
       </c>
@@ -2500,8 +4271,12 @@
       <c r="C37" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+      <c r="D37" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F37" s="7"/>
       <c r="G37" s="5">
         <f t="shared" si="0"/>
@@ -2513,11 +4288,11 @@
       </c>
       <c r="I37" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="5">
         <f t="shared" si="4"/>
@@ -2525,10 +4300,10 @@
       </c>
       <c r="L37" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:13">
       <c r="A38" s="7" t="s">
         <v>44</v>
       </c>
@@ -2538,9 +4313,15 @@
       <c r="C38" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G38" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2551,22 +4332,22 @@
       </c>
       <c r="I38" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:13" ht="30">
       <c r="A39" s="7" t="s">
         <v>45</v>
       </c>
@@ -2576,9 +4357,15 @@
       <c r="C39" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G39" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2589,22 +4376,25 @@
       </c>
       <c r="I39" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:13">
       <c r="A40" s="7" t="s">
         <v>46</v>
       </c>
@@ -2614,8 +4404,12 @@
       <c r="C40" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
+      <c r="D40" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F40" s="7"/>
       <c r="G40" s="5">
         <f t="shared" si="0"/>
@@ -2627,11 +4421,11 @@
       </c>
       <c r="I40" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="5">
         <f t="shared" si="4"/>
@@ -2639,10 +4433,10 @@
       </c>
       <c r="L40" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:13">
       <c r="A41" s="7" t="s">
         <v>47</v>
       </c>
@@ -2686,7 +4480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:13">
       <c r="A42" s="15" t="s">
         <v>17</v>
       </c>
@@ -2730,7 +4524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:13">
       <c r="A43" s="7" t="s">
         <v>18</v>
       </c>
@@ -2740,9 +4534,15 @@
       <c r="C43" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G43" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2753,22 +4553,22 @@
       </c>
       <c r="I43" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L43" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:13">
       <c r="A44" s="7" t="s">
         <v>19</v>
       </c>
@@ -2778,8 +4578,12 @@
       <c r="C44" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
+      <c r="D44" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F44" s="7"/>
       <c r="G44" s="5">
         <f t="shared" si="0"/>
@@ -2791,11 +4595,11 @@
       </c>
       <c r="I44" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="5">
         <f t="shared" si="4"/>
@@ -2803,10 +4607,10 @@
       </c>
       <c r="L44" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:13">
       <c r="A45" s="7" t="s">
         <v>48</v>
       </c>
@@ -2819,8 +4623,12 @@
       <c r="D45" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="E45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G45" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2835,18 +4643,18 @@
       </c>
       <c r="J45" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" s="6">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:13">
       <c r="A46" s="7" t="s">
         <v>20</v>
       </c>
@@ -2862,7 +4670,9 @@
       <c r="E46" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="G46" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2881,14 +4691,14 @@
       </c>
       <c r="K46" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="6">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:13">
       <c r="A47" s="16" t="s">
         <v>21</v>
       </c>
@@ -2896,7 +4706,9 @@
       <c r="C47" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="7"/>
+      <c r="D47" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="5">
@@ -2909,7 +4721,7 @@
       </c>
       <c r="I47" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="5">
         <f t="shared" si="3"/>
@@ -2921,10 +4733,13 @@
       </c>
       <c r="L47" s="6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M47" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:13">
       <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
@@ -2934,8 +4749,12 @@
       <c r="C48" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
+      <c r="D48" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F48" s="7"/>
       <c r="G48" s="5">
         <f t="shared" si="0"/>
@@ -2947,11 +4766,11 @@
       </c>
       <c r="I48" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="5">
         <f t="shared" si="4"/>
@@ -2959,7 +4778,7 @@
       </c>
       <c r="L48" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2972,8 +4791,12 @@
       <c r="C49" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="D49" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F49" s="7"/>
       <c r="G49" s="5">
         <f t="shared" si="0"/>
@@ -2985,11 +4808,11 @@
       </c>
       <c r="I49" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" s="5">
         <f t="shared" si="4"/>
@@ -2997,7 +4820,7 @@
       </c>
       <c r="L49" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3010,7 +4833,9 @@
       <c r="C50" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="7"/>
+      <c r="D50" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="5">
@@ -3023,7 +4848,7 @@
       </c>
       <c r="I50" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" s="5">
         <f t="shared" si="3"/>
@@ -3035,7 +4860,7 @@
       </c>
       <c r="L50" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3048,8 +4873,12 @@
       <c r="C51" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
+      <c r="D51" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F51" s="7"/>
       <c r="G51" s="5">
         <f t="shared" si="0"/>
@@ -3061,11 +4890,11 @@
       </c>
       <c r="I51" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" s="5">
         <f t="shared" si="4"/>
@@ -3073,7 +4902,7 @@
       </c>
       <c r="L51" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3086,8 +4915,12 @@
       <c r="C52" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
+      <c r="D52" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F52" s="7"/>
       <c r="G52" s="5">
         <f t="shared" si="0"/>
@@ -3099,11 +4932,11 @@
       </c>
       <c r="I52" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="5">
         <f t="shared" si="4"/>
@@ -3111,7 +4944,7 @@
       </c>
       <c r="L52" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3124,8 +4957,12 @@
       <c r="C53" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
+      <c r="D53" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F53" s="7"/>
       <c r="G53" s="5">
         <f t="shared" si="0"/>
@@ -3137,11 +4974,11 @@
       </c>
       <c r="I53" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" s="5">
         <f t="shared" si="4"/>
@@ -3149,7 +4986,7 @@
       </c>
       <c r="L53" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3162,9 +4999,15 @@
       <c r="C54" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
+      <c r="D54" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G54" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3175,19 +5018,19 @@
       </c>
       <c r="I54" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3200,8 +5043,12 @@
       <c r="C55" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
+      <c r="D55" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="F55" s="7"/>
       <c r="G55" s="5">
         <f t="shared" si="0"/>
@@ -3213,11 +5060,11 @@
       </c>
       <c r="I55" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55" s="5">
         <f t="shared" si="4"/>
@@ -3225,7 +5072,7 @@
       </c>
       <c r="L55" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3238,8 +5085,12 @@
       <c r="C56" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
+      <c r="D56" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="F56" s="7"/>
       <c r="G56" s="5">
         <f t="shared" si="0"/>
@@ -3251,11 +5102,11 @@
       </c>
       <c r="I56" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" s="5">
         <f t="shared" si="4"/>
@@ -3263,75 +5114,395 @@
       </c>
       <c r="L56" s="6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:H56">
     <sortCondition ref="A2:A56"/>
   </sortState>
-  <conditionalFormatting sqref="B47 B55 B27:F27 B4 B8:F8 B6 C7:F7 B36:F36 B17:B18 F14 B39:F39 D13:F13 C5:F5 C37:F38 C15:F16 C48:F48 C20:F20 F18 C23:F23 C29:F29 E45:F45 D52:F52 C53:F54 C56:F56 B30:F30 C25:F25 D24:F24 D19:F19 C34:F34 D55:F55 B28 D28:F28 C44:F44 D43:F43 D35:F35 F46 D3:F4 C51:F51 B31 D31:F33 D49:F50 C9:F12 D22:F22 D47:F47 D26:F26 C40:F42">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="17">
+  <conditionalFormatting sqref="B47 B55 B4 B8:C8 B6 C7 B17:B18 B39:C39 C48 C20:F20 C23 F52 C56 F18:F19 B28 C44 B31 E50:F50 D3:F3 C5:F5 C9:F11 C15:F15 D22:F22 C25:F25 D26:F26 B27:F27 C29:F29 B30:F30 D31:F33 C34:F34 D35:F35 B36:F36 C38:F38 C40:F42 D43:F43 C51:F51 D55:F55 C53:F53 F4 F7:F8 C12 F12:F14 C16 F16 F24 C37 F37 E45:F45 F44:F46 E47:F47 F48:F49 C54:E54 F56">
+    <cfRule type="notContainsBlanks" dxfId="175" priority="97">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="18" priority="18">
+    <cfRule type="containsBlanks" dxfId="174" priority="98">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="173" priority="95">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="16" priority="16">
+    <cfRule type="containsBlanks" dxfId="172" priority="96">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="171" priority="93">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="14" priority="14">
+    <cfRule type="containsBlanks" dxfId="170" priority="94">
       <formula>LEN(TRIM(B10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:E14">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="169" priority="91">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="12" priority="12">
+    <cfRule type="containsBlanks" dxfId="168" priority="92">
       <formula>LEN(TRIM(B14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:D17">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="167" priority="89">
       <formula>LEN(TRIM(C17))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="10" priority="10">
+    <cfRule type="containsBlanks" dxfId="166" priority="90">
       <formula>LEN(TRIM(C17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="165" priority="85">
       <formula>LEN(TRIM(B46))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="164" priority="86">
       <formula>LEN(TRIM(B46))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="163" priority="83">
       <formula>LEN(TRIM(B54))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="162" priority="84">
       <formula>LEN(TRIM(B54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="161" priority="81">
       <formula>LEN(TRIM(B29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
+    <cfRule type="containsBlanks" dxfId="160" priority="82">
       <formula>LEN(TRIM(B29))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="notContainsBlanks" dxfId="159" priority="79">
+      <formula>LEN(TRIM(D4))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="158" priority="80">
+      <formula>LEN(TRIM(D4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="notContainsBlanks" dxfId="155" priority="77">
+      <formula>LEN(TRIM(E4))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="154" priority="78">
+      <formula>LEN(TRIM(E4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="notContainsBlanks" dxfId="151" priority="75">
+      <formula>LEN(TRIM(D7))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="150" priority="76">
+      <formula>LEN(TRIM(D7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="notContainsBlanks" dxfId="147" priority="73">
+      <formula>LEN(TRIM(E7))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="146" priority="74">
+      <formula>LEN(TRIM(E7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="notContainsBlanks" dxfId="143" priority="71">
+      <formula>LEN(TRIM(D8))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="142" priority="72">
+      <formula>LEN(TRIM(D8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="notContainsBlanks" dxfId="139" priority="69">
+      <formula>LEN(TRIM(E8))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="138" priority="70">
+      <formula>LEN(TRIM(E8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="notContainsBlanks" dxfId="135" priority="67">
+      <formula>LEN(TRIM(D12))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="134" priority="68">
+      <formula>LEN(TRIM(D12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="notContainsBlanks" dxfId="131" priority="65">
+      <formula>LEN(TRIM(E12))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="130" priority="66">
+      <formula>LEN(TRIM(E12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="notContainsBlanks" dxfId="127" priority="63">
+      <formula>LEN(TRIM(D13))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="126" priority="64">
+      <formula>LEN(TRIM(D13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="notContainsBlanks" dxfId="123" priority="61">
+      <formula>LEN(TRIM(E13))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="122" priority="62">
+      <formula>LEN(TRIM(E13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="notContainsBlanks" dxfId="119" priority="59">
+      <formula>LEN(TRIM(D16))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="118" priority="60">
+      <formula>LEN(TRIM(D16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="57">
+      <formula>LEN(TRIM(E16))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="114" priority="58">
+      <formula>LEN(TRIM(E16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="55">
+      <formula>LEN(TRIM(D19))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="110" priority="56">
+      <formula>LEN(TRIM(D19))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="53">
+      <formula>LEN(TRIM(E19))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="106" priority="54">
+      <formula>LEN(TRIM(E19))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="notContainsBlanks" dxfId="103" priority="51">
+      <formula>LEN(TRIM(D23))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="102" priority="52">
+      <formula>LEN(TRIM(D23))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="notContainsBlanks" dxfId="99" priority="49">
+      <formula>LEN(TRIM(E23))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="98" priority="50">
+      <formula>LEN(TRIM(E23))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="47">
+      <formula>LEN(TRIM(F23))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="94" priority="48">
+      <formula>LEN(TRIM(F23))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="notContainsBlanks" dxfId="91" priority="45">
+      <formula>LEN(TRIM(E24))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="90" priority="46">
+      <formula>LEN(TRIM(E24))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="43">
+      <formula>LEN(TRIM(D24))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="86" priority="44">
+      <formula>LEN(TRIM(D24))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="41">
+      <formula>LEN(TRIM(D28))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="82" priority="42">
+      <formula>LEN(TRIM(D28))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="39">
+      <formula>LEN(TRIM(E28))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="78" priority="40">
+      <formula>LEN(TRIM(E28))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="37">
+      <formula>LEN(TRIM(F28))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="74" priority="38">
+      <formula>LEN(TRIM(F28))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="35">
+      <formula>LEN(TRIM(D37))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="70" priority="36">
+      <formula>LEN(TRIM(D37))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="33">
+      <formula>LEN(TRIM(E37))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="66" priority="34">
+      <formula>LEN(TRIM(E37))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="31">
+      <formula>LEN(TRIM(D39))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="62" priority="32">
+      <formula>LEN(TRIM(D39))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="29">
+      <formula>LEN(TRIM(E39))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="58" priority="30">
+      <formula>LEN(TRIM(E39))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="27">
+      <formula>LEN(TRIM(F39))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="54" priority="28">
+      <formula>LEN(TRIM(F39))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="25">
+      <formula>LEN(TRIM(D44))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="50" priority="26">
+      <formula>LEN(TRIM(D44))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="23">
+      <formula>LEN(TRIM(E44))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="46" priority="24">
+      <formula>LEN(TRIM(E44))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="21">
+      <formula>LEN(TRIM(D47))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="42" priority="22">
+      <formula>LEN(TRIM(D47))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="19">
+      <formula>LEN(TRIM(D48))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="38" priority="20">
+      <formula>LEN(TRIM(D48))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="17">
+      <formula>LEN(TRIM(E48))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="34" priority="18">
+      <formula>LEN(TRIM(E48))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="15">
+      <formula>LEN(TRIM(D49))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="30" priority="16">
+      <formula>LEN(TRIM(D49))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="13">
+      <formula>LEN(TRIM(E49))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="26" priority="14">
+      <formula>LEN(TRIM(E49))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="11">
+      <formula>LEN(TRIM(D50))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="22" priority="12">
+      <formula>LEN(TRIM(D50))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="9">
+      <formula>LEN(TRIM(D52))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="18" priority="10">
+      <formula>LEN(TRIM(D52))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="7">
+      <formula>LEN(TRIM(E52))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="14" priority="8">
+      <formula>LEN(TRIM(E52))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F54">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="5">
+      <formula>LEN(TRIM(F54))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="10" priority="6">
+      <formula>LEN(TRIM(F54))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="3">
+      <formula>LEN(TRIM(D56))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
+      <formula>LEN(TRIM(D56))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
+      <formula>LEN(TRIM(E56))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
+      <formula>LEN(TRIM(E56))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>